<commit_message>
Spotiy source code change
</commit_message>
<xml_diff>
--- a/Book11.xlsx
+++ b/Book11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F125"/>
+  <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,11 @@
           <t>TITLE</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>NEW PLAYS June 24, 2024</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -471,11 +476,7 @@
           <t>https://open.spotify.com/track/19Y2KyC2lT8m6O6W9nIgc1?si=4ceeac33586e427c</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
           <t>2022-10-25</t>
@@ -494,6 +495,11 @@
       <c r="F2" t="inlineStr">
         <is>
           <t>Darshan Dihi Dinanath</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -528,6 +534,11 @@
           <t>Satnam Waheguru</t>
         </is>
       </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>187,266</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -560,6 +571,11 @@
           <t>Ik Onkaar</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>4,514</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -567,11 +583,7 @@
           <t>https://open.spotify.com/track/6ZnNesqZbG6hk5kYrqxrZ2?si=3dabd12de3864564</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
           <t>2013-07-16</t>
@@ -590,6 +602,11 @@
       <c r="F5" t="inlineStr">
         <is>
           <t>Sainatha Sainatha</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -599,11 +616,7 @@
           <t>https://open.spotify.com/track/4YwZndGgej407LFm4RBWwM?si=eeec6729268b4588</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
           <t>2023-12-13</t>
@@ -622,6 +635,11 @@
       <c r="F6" t="inlineStr">
         <is>
           <t>Om Sai Ram</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -656,6 +674,11 @@
           <t>Sur Ke Ghungroo</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>56,804</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -688,6 +711,11 @@
           <t>Radhe Radhe</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>3,793</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -720,6 +748,11 @@
           <t>Argalastotra</t>
         </is>
       </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>6,857</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -752,6 +785,11 @@
           <t>Shree Datta Bavani</t>
         </is>
       </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>1,119</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -784,6 +822,11 @@
           <t>Achyutam Keshavam</t>
         </is>
       </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>23,912</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -791,11 +834,7 @@
           <t>https://open.spotify.com/track/1dzFIjCrE16dzd2J55cPRx?si=41d48c7186a64f02</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
           <t>2022-12-22</t>
@@ -814,6 +853,11 @@
       <c r="F12" t="inlineStr">
         <is>
           <t>Om Sai Jai Sai</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -823,29 +867,30 @@
           <t>https://open.spotify.com/track/5kxNZ0CG58rUz4b0cXCjPH?si=e7b737dbda434baa</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2022-12-30</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Vidhi Sharma</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>© 2022 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Ambe Bhawani</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -855,29 +900,30 @@
           <t>https://open.spotify.com/track/2xBMthE3IKrDAzsk2WYxOi?si=2bc38cc26dea4b12</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2023-01-01</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Akshay Acharya</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>© 2022 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Gajanana Gananayaka</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -894,22 +940,27 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2023-01-03</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Raghav Sachar</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>© 2022 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Hanuman Chalisa</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -919,29 +970,30 @@
           <t>https://open.spotify.com/track/2S7SanMKPexdL7xLHIqqmb?si=0ad41f3e7738454a</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2023-01-11</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Dr. Rahul Joshi</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Shree Ramchandra Krupalu</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -958,22 +1010,27 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2023-01-17</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Sooryagayathri</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Naam Japan Kyu Chod Diya</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -983,29 +1040,30 @@
           <t>https://open.spotify.com/track/32qK3mJZWIcF3UgiQL6THZ?si=8f8e51ec6e444254</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2023-01-24</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Dr Sanjayraj Gaurinandan (SRG)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Ganesh Mantra Psytrance</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1015,29 +1073,30 @@
           <t>https://open.spotify.com/track/7BRHUpPQ552LPJ7Kxg53F8?si=d875c18e9c784b2b</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2023-01-25</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Uma Mohan</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Ashtavinayaka</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1047,29 +1106,30 @@
           <t>https://open.spotify.com/track/16EArYVJFfjRhCxta8bTO1?si=51d7f17b35f84131</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2023-02-06</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Uma Mohan</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Shiv Manas Puja</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1086,22 +1146,27 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2023-02-09</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Abhilipsa Panda, Arabinda Neog, JUNO</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Shiv Shiv Hai</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1118,22 +1183,27 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2023-02-13</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Malini Awasthi</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Shiv Tandav Stotra Hindi</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1150,22 +1220,27 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2023-02-15</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Uthara Unnikrishnan, Prithvi Chandrasekhar</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Karpura Gauram</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1182,22 +1257,27 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2009-09-11</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Swagatalakshmi Dasgupta</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>© 2009 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Keelakastaba</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1207,29 +1287,30 @@
           <t>https://open.spotify.com/track/14NSavEPFgyqnB6UxoYgAf?si=a8f63a86121148bc</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2023-02-27</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Vidhi Sharma</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Aigiri Nandini</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1246,22 +1327,27 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2023-03-02</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Shilpi Raj</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Ae Kanha Ji</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1271,29 +1357,30 @@
           <t>https://open.spotify.com/track/19Nx6UJpgJXx2A6OlbPjOV?si=387b7409f1d84266</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2023-03-03</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Uma Mohan</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Madhurashtakam</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1303,29 +1390,30 @@
           <t>https://open.spotify.com/track/6FjVqZTDNloR883BhCbCpy?si=35d08c7d58774cc8</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2023-03-04</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Hema Malini</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>© 2023 N A Classical</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Shyam Rang Mein</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1335,29 +1423,30 @@
           <t>https://open.spotify.com/track/2atAYlefDK56LaLlyF5bhN?si=effdea1f628e4711</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2023-03-04</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Hema Malini</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>© 2023 N A Classical</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Achyutam Keshavam</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1367,29 +1456,30 @@
           <t>https://open.spotify.com/track/5Lqqr9xBz6zpNsrk2s9Tbt?si=c7e6e71cf8c34935</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2015-09-05</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Shobha Ramesh</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>© 2015 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Haribolo Haribolo</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1406,22 +1496,27 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2009-09-11</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Swagatalakshmi Dasgupta</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>© 2009 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Chapter 13-devi Barpradan &amp; Devishukta</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1438,22 +1533,27 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2023-03-16</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Antara Nandy</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Dattatreya Stotram</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1470,22 +1570,27 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2023-03-18</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Sooryagayathri</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Hanuman Ashtak</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1502,22 +1607,27 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2023-03-21</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Abhilipsa Panda</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Hanuman Chalisa</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1534,22 +1644,27 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2023-03-29</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Malini Awasthi</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Chalo Ayodhya Dham</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1566,22 +1681,27 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2023-04-14</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Shreyas Puranik</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Radhe Shyam Bolo</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1591,29 +1711,30 @@
           <t>https://open.spotify.com/track/3yOQSnuAB25rf2UIMtNhI0?si=94212c7ad449468b</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2023-04-28</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Kumar Vishu</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Maa Meri Maa</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1630,22 +1751,27 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2023-05-31</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Abhilipsa Panda, Arabinda Neog, JUNO</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Hari Krishna</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1662,22 +1788,27 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2023-06-07</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Sooryagayathri, Ajay-Atul</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Pranamya Shirasa Devam</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1687,29 +1818,30 @@
           <t>https://open.spotify.com/track/24jOPYYMKo0bym56jDQaCY?si=60e70840601a4868</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2023-06-09</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Tushar Verma</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Maa Mansa Devi</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1719,29 +1851,30 @@
           <t>https://open.spotify.com/track/0NWFnPWeNus7qecyFNCYzr?si=49e4deec9b274587</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2023-06-14</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Hrishikesh Ranade</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Dindi Nighe Pandharisii</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1751,29 +1884,30 @@
           <t>https://open.spotify.com/track/0zTOdPXMQECHhVnzpGv77A?si=5d114d52febf4d44</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2023-06-16</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Lakhvir Rinku Bagwali</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Sun Lai Maa Ardaas</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1790,22 +1924,27 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2023-06-20</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Abhilipsa Panda, Sri Siba Rath</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Jagannath Stuti</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1822,22 +1961,27 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2023-06-20</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Abhilipsa Panda</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Niladri Natham</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1854,22 +1998,27 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2023-06-20</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Abhilipsa Panda, Sri Siba Rath</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Putapayodhi</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1886,22 +2035,27 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2023-06-20</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Abhilipsa Panda</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Ghana Sundara</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1918,22 +2072,27 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2023-06-21</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Uma Mohan, Dr. Prema Shanker</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Brahma Tat Tvam Asi</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1950,22 +2109,27 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2023-06-21</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Adarsh Shinde, Apurva Nisshad</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Majha Vithuraya</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1982,22 +2146,27 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2023-06-20</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Sri Siba Rath</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Dehi Padapallabh</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2014,22 +2183,27 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2023-06-20</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Sri Siba Rath</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Ehi Murare Kunj Bihare</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2046,22 +2220,27 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2023-06-26</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Pratibha Singh Baghel</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Shiv Vandana</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2071,29 +2250,30 @@
           <t>https://open.spotify.com/track/4pTKuOQs0FcQeBglMFIfe8?si=1d99a2448fab47fc</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2023-06-20</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Hrishikesh Ranade</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Parabrahma Aale Gaa</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2110,22 +2290,27 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2023-07-04</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Sonu Nigam, Shreyas Puranik</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Mahadeva</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2135,29 +2320,30 @@
           <t>https://open.spotify.com/track/3Fs8UDiQ8vf7zXYIsj5rhu?si=c095d65db7194470</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2023-07-10</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Antara Nandy</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Bam Bam Bam Bhole</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2174,22 +2360,27 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2023-07-17</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Sooryagayathri</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Namaskarartha Shiv Mantra</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2206,22 +2397,27 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2011-07-29</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Malini Awasthi</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>© 2011 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Amma Mere Baba Ko</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2238,22 +2434,27 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2023-07-24</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Abhilipsa Panda, Shreyas Puranik</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Bam Bhole Bam</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2263,29 +2464,30 @@
           <t>https://open.spotify.com/track/1EofVUGuQU1KkSAiXLp2Ny?si=486396c049764933</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2023-07-26</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Pratibha Singh Baghel</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Shiv Om Hari Om</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2295,29 +2497,30 @@
           <t>https://open.spotify.com/track/6Yeb5B5MGnsqK20VLv10pc?si=62b343b1a17140b8</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2023-07-27</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Rahul Babbar</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Kanha</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2327,29 +2530,30 @@
           <t>https://open.spotify.com/track/59cbPEnGjjUHdQSCHKTa88?si=e320030923bb4eda</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2023-07-28</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Gitanshi Tiwari Geet</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Baandh Sehra Aaye Kailasha</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2359,29 +2563,30 @@
           <t>https://open.spotify.com/track/6Vu7YeoxwufL6ch27mumV6?si=8b6b93ccf79a4352</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2011-07-29</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Malini Awasthi</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>© 2011 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Sawan Jhadi Lagi</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2398,22 +2603,27 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2023-08-04</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Anuradha Paudwal</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Ganesh Pancharatna</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2430,22 +2640,27 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2023-08-07</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Shekhar Jaiswal</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Mere Baba Bholenath</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2462,22 +2677,27 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2023-07-31</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Uthara Unnikrishnan</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Chandrashekhar Stotram</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2487,29 +2707,30 @@
           <t>https://open.spotify.com/track/7sPm5VJVqMDEGRXrJhaPmW?si=fb514261347e4a48</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2023-08-21</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Ratika Johri</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Shiv Shambhu</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2526,22 +2747,27 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2023-08-23</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Divya Kumar, Raghav Sachar</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Krishna Krishna</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2558,22 +2784,27 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2023-08-28</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Rahul Vellal</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Shiv Raksha Stotra</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2583,29 +2814,30 @@
           <t>https://open.spotify.com/track/4FZ2xv7TdOgCiIKtjJTw4M?si=18188fe3faf9481b</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2023-08-30</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Calcutta K Srividya, Mohan Kannan</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Govinda Nandanandana</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2615,29 +2847,30 @@
           <t>https://open.spotify.com/track/5QCXoQlJirA8JNgFy0yKSo?si=7bc25acac3d04837</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr">
         <is>
-          <t>2023-08-31</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Antara Nandy</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Roop Hari Ka</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2647,29 +2880,30 @@
           <t>https://open.spotify.com/track/5YxAEn54RHKIpOWY4J2kLj?si=aadbd4060eff458a</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr">
         <is>
-          <t>2023-09-01</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Malini Awasthi</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Kanha Padharo</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2679,29 +2913,30 @@
           <t>https://open.spotify.com/track/10QCLQqptHovJjzV6E7HlZ?si=f60110e9be9649ae</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr">
         <is>
-          <t>2023-09-02</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Vaishnavi Sharma</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Achyutam Keshavam</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2711,29 +2946,30 @@
           <t>https://open.spotify.com/track/7jBSUIpqCko6Nwlkuq9Ry7?si=5e26901628554236</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr">
         <is>
-          <t>2023-09-04</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Hema Malini</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>© 2023 N A Classical</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Jhoola Jhoole Radha Rani</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2743,29 +2979,30 @@
           <t>https://open.spotify.com/track/4QjCXTLNvomak0oR8p7nLL?si=5ba034ca10fc4c6b</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr">
         <is>
-          <t>2023-09-06</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Uthara Unnikrishnan</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Krishna Hare Govinda Hare</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2782,22 +3019,27 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>2023-09-06</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Sonu Nigam</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>O Govinda</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2814,22 +3056,27 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>2023-09-08</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Shankar Mahadevan, Akshay Purandare, Manoj Yadav</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Gajamukha</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2846,22 +3093,27 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>2023-09-09</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Sharayu Date, Akshay Purandare, Manoj Yadav</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Mayureshwara</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2878,22 +3130,27 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>2023-09-12</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Abhilipsa Panda, Rohan Puntambekar</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Deva Ganesha</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2910,22 +3167,27 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>2023-09-13</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Abhay Jodhpurkar, Akshay Purandare, Manoj Yadav</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>© 2023 Nupur Audio</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Sukhakarta Deva</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2942,22 +3204,27 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>2023-09-14</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Shankar Mahadevan</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Shree Ganeshji Aaye</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -2974,22 +3241,27 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>2023-09-15</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Sooryagayathri</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Ganesh Namo</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3006,22 +3278,27 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>2023-09-16</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Uthara Unnikrishnan</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Sukhakarta Gajanan</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3038,22 +3315,27 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>2023-09-18</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Shweta Mohan</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Ganeshay Dheemahi</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3063,29 +3345,30 @@
           <t>https://open.spotify.com/track/04rrl1cCL82gbors5U1HX1?si=93b135f4eb2949ab</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B83" t="inlineStr"/>
       <c r="C83" t="inlineStr">
         <is>
-          <t>2023-09-17</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Riya Borse</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Gan Gan Ganpati</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3102,22 +3385,27 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>2012-08-29</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Chorus</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>© 2012 Anuradha Paudwal And Aditya Paudwal</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Morayaa Re Bappa</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3127,29 +3415,30 @@
           <t>https://open.spotify.com/track/6jEDxjn1AxTMuCNusSpMQg?si=3a6ea7228dc64632</t>
         </is>
       </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B85" t="inlineStr"/>
       <c r="C85" t="inlineStr">
         <is>
-          <t>2023-09-15</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Keval Walanj</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Dev Majha Bappa</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3159,29 +3448,30 @@
           <t>https://open.spotify.com/track/0jwTuDO4QAGBMK3NymIHhT?si=74c2eec89c804951</t>
         </is>
       </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B86" t="inlineStr"/>
       <c r="C86" t="inlineStr">
         <is>
-          <t>2023-09-22</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Nikita Rai</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Gananayakaya</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3191,29 +3481,30 @@
           <t>https://open.spotify.com/track/0BuAcKXfVSwBXxfds3L3ez?si=c0bb3ab781ed4920</t>
         </is>
       </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B87" t="inlineStr"/>
       <c r="C87" t="inlineStr">
         <is>
-          <t>2023-09-25</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Ratika Johri</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Ganpati Tu</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3230,22 +3521,27 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>2023-09-26</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Abhilipsa Panda, Rohan Puntambekar</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Ghalin Lotangan</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3262,22 +3558,27 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>2023-10-05</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Anuradha Paudwal</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Hey Ram Shri Ram</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3287,29 +3588,30 @@
           <t>https://open.spotify.com/track/134WwF5wYkO0GeYmHJVttw?si=a77543c93c6e40d0</t>
         </is>
       </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B90" t="inlineStr"/>
       <c r="C90" t="inlineStr">
         <is>
-          <t>2023-09-05</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>L. Nitesh Kumar</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Shree Krishna Mahamantra</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3319,29 +3621,30 @@
           <t>https://open.spotify.com/track/5PFUAmjL39d4sZNmJnbQZl?si=6052998e7da04cb3</t>
         </is>
       </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B91" t="inlineStr"/>
       <c r="C91" t="inlineStr">
         <is>
-          <t>2023-10-09</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Malini Awasthi</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Jagdambe Maa</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3358,22 +3661,27 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>2023-10-12</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Lakhbir Singh Lakkha</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Ambe Niwas</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3383,29 +3691,30 @@
           <t>https://open.spotify.com/track/0BBw4nniBoYON8MC7eZGG7?si=4f4c816c09974ef7</t>
         </is>
       </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B93" t="inlineStr"/>
       <c r="C93" t="inlineStr">
         <is>
-          <t>2023-10-13</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>DS Pal</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Navdurga Avtar Katha</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3422,22 +3731,27 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>2023-10-14</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Abhilipsa Panda, Rohan Puntambekar</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Maa Durga Anthem</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3454,22 +3768,27 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>2023-10-15</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Alka Yagnik</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Bhor Bhayi</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3479,29 +3798,30 @@
           <t>https://open.spotify.com/track/7EZx7qt2BnxI1kzOpTl0Kn?si=90282ef588694beb</t>
         </is>
       </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B96" t="inlineStr"/>
       <c r="C96" t="inlineStr">
         <is>
-          <t>2023-10-15</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Vidhi Sharma</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Shri Durga Shailputri Stavan</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3511,29 +3831,30 @@
           <t>https://open.spotify.com/track/4BG9PG7BDNzXGG2Wx6O2Tr?si=32f8b71353054138</t>
         </is>
       </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B97" t="inlineStr"/>
       <c r="C97" t="inlineStr">
         <is>
-          <t>2023-10-17</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Vidhi Sharma</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Shri Durga Chandraghanta Stavan</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3550,22 +3871,27 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>2023-10-17</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Lakhbir Singh Lakkha</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Sher Sawari Kardi</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3575,29 +3901,30 @@
           <t>https://open.spotify.com/track/1tXH9vVkxdSqgqKgYa7SIa?si=431fe8ba75f64cdb</t>
         </is>
       </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B99" t="inlineStr"/>
       <c r="C99" t="inlineStr">
         <is>
-          <t>2023-10-18</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Vidhi Sharma</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Shri Durga Kushmanda Stavan</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3607,29 +3934,30 @@
           <t>https://open.spotify.com/track/4ydLbdY7VVanSwwRuUpSfD?si=bad8a290a2404f26</t>
         </is>
       </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B100" t="inlineStr"/>
       <c r="C100" t="inlineStr">
         <is>
-          <t>2023-10-19</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Vidhi Sharma</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Shri Durga Skandamata Stavan</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3639,29 +3967,30 @@
           <t>https://open.spotify.com/track/3OjGPCBur0X7jwIWrYFVfH?si=385c73332eca4971</t>
         </is>
       </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B101" t="inlineStr"/>
       <c r="C101" t="inlineStr">
         <is>
-          <t>2023-10-20</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Vidhi Sharma</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Shri Durga Katyayani Stavan</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3678,22 +4007,27 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>2023-10-20</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Rajalakshmee Sanjay</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Aigiri Nandini - Hindi</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3703,29 +4037,30 @@
           <t>https://open.spotify.com/track/4cZasm1q46g3m6bZyy6g5I?si=46b763a26e23465f</t>
         </is>
       </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B103" t="inlineStr"/>
       <c r="C103" t="inlineStr">
         <is>
-          <t>2023-10-21</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Vidhi Sharma</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Shri Durga Kaal Ratri Stavan</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3735,29 +4070,30 @@
           <t>https://open.spotify.com/track/4Pp4KbsjhJR1jXYjjOp3fX?si=5887e6db89a04104</t>
         </is>
       </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B104" t="inlineStr"/>
       <c r="C104" t="inlineStr">
         <is>
-          <t>2023-10-22</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Vidhi Sharma</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Shri Durga Mahagauri Stavan</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3767,29 +4103,30 @@
           <t>https://open.spotify.com/track/24QLB1IbvZmJR3ePZPqOq7?si=e98367ad093b49b9</t>
         </is>
       </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B105" t="inlineStr"/>
       <c r="C105" t="inlineStr">
         <is>
-          <t>2023-10-23</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Vidhi Sharma</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>Shri Durga Siddhidatri Stavan</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3799,29 +4136,30 @@
           <t>https://open.spotify.com/track/2z94r1WHKijm3digvH3EfX?si=ff366fbb8dee4f7f</t>
         </is>
       </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B106" t="inlineStr"/>
       <c r="C106" t="inlineStr">
         <is>
-          <t>2023-10-24</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Vidhi Sharma</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Navdurga Aarti</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3831,29 +4169,30 @@
           <t>https://open.spotify.com/track/44zBPEmgHej23PrQ0ldwG7?si=0065fbf3e7114d57</t>
         </is>
       </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B107" t="inlineStr"/>
       <c r="C107" t="inlineStr">
         <is>
-          <t>2023-10-24</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Rahul Vellal</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Bhaye Pragat Kripala</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3870,22 +4209,27 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>2022-10-14</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Maithili Thakur</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>© 2022 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>Mahalakshmi Ashtak</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3902,22 +4246,27 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>2023-11-05</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Rahul Deshpande</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>Ram Raksha Stotra</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3927,29 +4276,30 @@
           <t>https://open.spotify.com/track/3lj0h2WbHDJKQC4UOJY1Xv?si=6be76af07aac4bf0</t>
         </is>
       </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B110" t="inlineStr"/>
       <c r="C110" t="inlineStr">
         <is>
-          <t>2023-11-06</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Devaki Pandit</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Devi Kavach</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3966,22 +4316,27 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>2023-11-08</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Sooryagayathri</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Ya Kundendu</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -3991,29 +4346,30 @@
           <t>https://open.spotify.com/track/5Ax22NBiDJDKp085QyBbVi?si=fe3f1e081cbd45d6</t>
         </is>
       </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B112" t="inlineStr"/>
       <c r="C112" t="inlineStr">
         <is>
-          <t>2023-11-09</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Vijay Prakash</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>Ganesh Laghu Stotra</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4030,22 +4386,27 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>2023-11-10</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Agam Aggarwal</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>Kuber Lakshmi Namami</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4062,22 +4423,27 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>2023-11-11</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>P. Unnikrishnan, Uthara Unnikrishnan</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>Japiye Sada Shri Ram</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4087,29 +4453,30 @@
           <t>https://open.spotify.com/track/3nXigcyYPzwvWoAhvZ2da0?si=2add4b215b56462b</t>
         </is>
       </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B115" t="inlineStr"/>
       <c r="C115" t="inlineStr">
         <is>
-          <t>2023-11-12</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Vinaya Karthik Rajan, Savithri Prithvi</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>Mahalakshmi Kavacham</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4119,29 +4486,30 @@
           <t>https://open.spotify.com/track/5lBOzMu9nIMjwWgd8ZfR6s?si=f0858af003384aff</t>
         </is>
       </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B116" t="inlineStr"/>
       <c r="C116" t="inlineStr">
         <is>
-          <t>2023-11-13</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Dr Sanjayraj Gaurinandan (SRG)</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>Psytrance Sai Mantra</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4151,29 +4519,30 @@
           <t>https://open.spotify.com/track/1VwOuHxB9NID0cEfztVuBS?si=406b92f9e7a74e69</t>
         </is>
       </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B117" t="inlineStr"/>
       <c r="C117" t="inlineStr">
         <is>
-          <t>2023-11-14</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Ratika Johri</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>Bolo Ram</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4190,22 +4559,27 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>2024-01-12</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Agam Aggarwal</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>© 2023 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>Surya Mahamantra</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4222,22 +4596,27 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>2024-01-29</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Shankar Mahadevan, Ranjin Raj, Shivala</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>© 2024 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>Shiva Shiva (From "Mahadev Ka Gorakhpur")</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4254,22 +4633,27 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>2024-02-05</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Akshay Kumar, Sudhir Yaduvanshi, Vikram Montrose</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>© 2024 Times Music &amp; Cape of Good Films LLP</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>Shambhu</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4286,22 +4670,27 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>2024-02-05</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Agam Aggarwal</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>© 2024 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>Mahadeva (From "Mahadev Ka Gorakhpur")</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4311,29 +4700,30 @@
           <t>https://open.spotify.com/track/6qSTg371XsCKisWqX6zpOu?si=befeec23d4374c21</t>
         </is>
       </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B122" t="inlineStr"/>
       <c r="C122" t="inlineStr">
         <is>
-          <t>2024-02-14</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Ajivasan Kids</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>© 2024 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>Ya Kundendu</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4350,22 +4740,27 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>2024-02-12</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Agam Aggarwal</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>© 2024 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>Woh Indra Jinki (From "Mahadev Ka Gorakhpur")</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4382,22 +4777,27 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>2024-02-21</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Shreya Ghoshal</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>© 2024 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>Morya Tumhara Gunjan Hai</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4407,29 +4807,30 @@
           <t>https://open.spotify.com/track/7EOOBw9P5lo9O5Dn6m5WY1?si=d9f6fd1d10414026</t>
         </is>
       </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="B125" t="inlineStr"/>
       <c r="C125" t="inlineStr">
         <is>
-          <t>2024-01-22</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Ajivasan Kids</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>© 2024 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>Ram Ram Jai Raja Ram</t>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
plays and labels fixed
</commit_message>
<xml_diff>
--- a/Book11.xlsx
+++ b/Book11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:H125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,11 @@
           <t>NEW PLAYS June 24, 2024</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>NEW PLAYS September 06, 2024</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -489,7 +494,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>© 2022 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -497,7 +502,8 @@
           <t>Darshan Dihi Dinanath</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -526,7 +532,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>© 2022 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -537,6 +543,11 @@
       <c r="G3" t="inlineStr">
         <is>
           <t>187,266</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>199,789</t>
         </is>
       </c>
     </row>
@@ -563,7 +574,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>© 2022 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -574,6 +585,11 @@
       <c r="G4" t="inlineStr">
         <is>
           <t>4,514</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>4,594</t>
         </is>
       </c>
     </row>
@@ -596,7 +612,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>© 2013 Alpha Digitech</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -604,7 +620,8 @@
           <t>Sainatha Sainatha</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -629,7 +646,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>© 2023 Krishna Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -637,7 +654,8 @@
           <t>Om Sai Ram</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -656,27 +674,32 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2022-11-16</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Maithili Thakur</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>© 2022 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Sur Ke Ghungroo</t>
+          <t>None</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
           <t>56,804</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -693,27 +716,32 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2022-11-30</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Vidhi Sharma</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>© 2022 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Radhe Radhe</t>
+          <t>None</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
           <t>3,793</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -730,27 +758,32 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2009-09-11</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Swagatalakshmi Dasgupta</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>© 2009 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Argalastotra</t>
+          <t>None</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
           <t>6,857</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -767,27 +800,32 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2022-12-03</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Anup Jalota, Dr. Rahul Joshi</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>© 2022 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Shree Datta Bavani</t>
+          <t>None</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
           <t>1,119</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -804,27 +842,32 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2022-12-08</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Sooryagayathri</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>© 2022 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Achyutam Keshavam</t>
+          <t>None</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
           <t>23,912</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -837,25 +880,26 @@
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2022-12-22</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Tripti Shakya</t>
+          <t>None</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>© 2022 Times Music</t>
+          <t>None</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Om Sai Jai Sai</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -888,7 +932,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -921,7 +966,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -958,7 +1004,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -991,7 +1038,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1028,7 +1076,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1061,7 +1110,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1094,7 +1144,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1127,7 +1178,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1164,7 +1216,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1201,7 +1254,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1238,7 +1292,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1275,7 +1330,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1308,7 +1364,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1345,7 +1402,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1378,7 +1436,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1411,7 +1470,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1444,7 +1504,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1477,7 +1538,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1514,7 +1576,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr">
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1551,7 +1614,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr">
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1588,7 +1652,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1625,7 +1690,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr">
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1662,7 +1728,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr">
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1699,7 +1766,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1732,7 +1800,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr">
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1769,7 +1838,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr">
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1806,7 +1876,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr">
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1839,7 +1910,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr">
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1872,7 +1944,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr">
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1905,7 +1978,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr">
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1942,7 +2016,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr">
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1979,7 +2054,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr">
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2016,7 +2092,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr">
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2053,7 +2130,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G46" t="inlineStr">
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2090,7 +2168,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G47" t="inlineStr">
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2127,7 +2206,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G48" t="inlineStr">
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2164,7 +2244,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr">
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2201,7 +2282,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G50" t="inlineStr">
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2238,7 +2320,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G51" t="inlineStr">
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2271,7 +2354,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G52" t="inlineStr">
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2308,7 +2392,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G53" t="inlineStr">
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2341,7 +2426,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G54" t="inlineStr">
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2378,7 +2464,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G55" t="inlineStr">
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2415,7 +2502,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G56" t="inlineStr">
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2452,7 +2540,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G57" t="inlineStr">
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2485,7 +2574,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G58" t="inlineStr">
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2518,7 +2608,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G59" t="inlineStr">
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2551,7 +2642,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G60" t="inlineStr">
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2584,7 +2676,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G61" t="inlineStr">
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2621,7 +2714,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G62" t="inlineStr">
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2658,7 +2752,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G63" t="inlineStr">
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2695,7 +2790,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G64" t="inlineStr">
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2728,7 +2824,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G65" t="inlineStr">
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2765,7 +2862,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G66" t="inlineStr">
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2802,7 +2900,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G67" t="inlineStr">
+      <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2835,7 +2934,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G68" t="inlineStr">
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2868,7 +2968,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G69" t="inlineStr">
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2901,7 +3002,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G70" t="inlineStr">
+      <c r="G70" t="inlineStr"/>
+      <c r="H70" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2934,7 +3036,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G71" t="inlineStr">
+      <c r="G71" t="inlineStr"/>
+      <c r="H71" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -2967,7 +3070,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G72" t="inlineStr">
+      <c r="G72" t="inlineStr"/>
+      <c r="H72" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3000,7 +3104,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G73" t="inlineStr">
+      <c r="G73" t="inlineStr"/>
+      <c r="H73" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3037,7 +3142,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G74" t="inlineStr">
+      <c r="G74" t="inlineStr"/>
+      <c r="H74" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3074,7 +3180,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G75" t="inlineStr">
+      <c r="G75" t="inlineStr"/>
+      <c r="H75" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3111,7 +3218,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G76" t="inlineStr">
+      <c r="G76" t="inlineStr"/>
+      <c r="H76" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3148,7 +3256,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G77" t="inlineStr">
+      <c r="G77" t="inlineStr"/>
+      <c r="H77" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3185,7 +3294,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G78" t="inlineStr">
+      <c r="G78" t="inlineStr"/>
+      <c r="H78" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3222,7 +3332,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G79" t="inlineStr">
+      <c r="G79" t="inlineStr"/>
+      <c r="H79" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3259,7 +3370,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G80" t="inlineStr">
+      <c r="G80" t="inlineStr"/>
+      <c r="H80" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3296,7 +3408,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G81" t="inlineStr">
+      <c r="G81" t="inlineStr"/>
+      <c r="H81" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3333,7 +3446,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G82" t="inlineStr">
+      <c r="G82" t="inlineStr"/>
+      <c r="H82" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3366,7 +3480,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G83" t="inlineStr">
+      <c r="G83" t="inlineStr"/>
+      <c r="H83" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3403,7 +3518,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G84" t="inlineStr">
+      <c r="G84" t="inlineStr"/>
+      <c r="H84" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3436,7 +3552,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G85" t="inlineStr">
+      <c r="G85" t="inlineStr"/>
+      <c r="H85" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3469,7 +3586,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G86" t="inlineStr">
+      <c r="G86" t="inlineStr"/>
+      <c r="H86" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3502,7 +3620,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G87" t="inlineStr">
+      <c r="G87" t="inlineStr"/>
+      <c r="H87" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3539,7 +3658,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G88" t="inlineStr">
+      <c r="G88" t="inlineStr"/>
+      <c r="H88" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3576,7 +3696,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G89" t="inlineStr">
+      <c r="G89" t="inlineStr"/>
+      <c r="H89" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3609,7 +3730,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G90" t="inlineStr">
+      <c r="G90" t="inlineStr"/>
+      <c r="H90" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3642,7 +3764,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G91" t="inlineStr">
+      <c r="G91" t="inlineStr"/>
+      <c r="H91" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3679,7 +3802,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G92" t="inlineStr">
+      <c r="G92" t="inlineStr"/>
+      <c r="H92" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3712,7 +3836,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G93" t="inlineStr">
+      <c r="G93" t="inlineStr"/>
+      <c r="H93" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3749,7 +3874,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G94" t="inlineStr">
+      <c r="G94" t="inlineStr"/>
+      <c r="H94" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3786,7 +3912,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G95" t="inlineStr">
+      <c r="G95" t="inlineStr"/>
+      <c r="H95" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3819,7 +3946,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G96" t="inlineStr">
+      <c r="G96" t="inlineStr"/>
+      <c r="H96" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3852,7 +3980,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G97" t="inlineStr">
+      <c r="G97" t="inlineStr"/>
+      <c r="H97" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3889,7 +4018,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G98" t="inlineStr">
+      <c r="G98" t="inlineStr"/>
+      <c r="H98" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3922,7 +4052,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G99" t="inlineStr">
+      <c r="G99" t="inlineStr"/>
+      <c r="H99" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3955,7 +4086,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G100" t="inlineStr">
+      <c r="G100" t="inlineStr"/>
+      <c r="H100" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3988,7 +4120,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G101" t="inlineStr">
+      <c r="G101" t="inlineStr"/>
+      <c r="H101" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4025,7 +4158,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G102" t="inlineStr">
+      <c r="G102" t="inlineStr"/>
+      <c r="H102" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4058,7 +4192,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G103" t="inlineStr">
+      <c r="G103" t="inlineStr"/>
+      <c r="H103" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4091,7 +4226,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G104" t="inlineStr">
+      <c r="G104" t="inlineStr"/>
+      <c r="H104" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4124,7 +4260,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G105" t="inlineStr">
+      <c r="G105" t="inlineStr"/>
+      <c r="H105" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4157,7 +4294,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G106" t="inlineStr">
+      <c r="G106" t="inlineStr"/>
+      <c r="H106" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4190,7 +4328,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G107" t="inlineStr">
+      <c r="G107" t="inlineStr"/>
+      <c r="H107" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4227,7 +4366,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G108" t="inlineStr">
+      <c r="G108" t="inlineStr"/>
+      <c r="H108" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4264,7 +4404,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G109" t="inlineStr">
+      <c r="G109" t="inlineStr"/>
+      <c r="H109" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4297,7 +4438,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G110" t="inlineStr">
+      <c r="G110" t="inlineStr"/>
+      <c r="H110" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4334,7 +4476,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G111" t="inlineStr">
+      <c r="G111" t="inlineStr"/>
+      <c r="H111" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4367,7 +4510,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G112" t="inlineStr">
+      <c r="G112" t="inlineStr"/>
+      <c r="H112" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4404,7 +4548,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G113" t="inlineStr">
+      <c r="G113" t="inlineStr"/>
+      <c r="H113" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4441,7 +4586,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G114" t="inlineStr">
+      <c r="G114" t="inlineStr"/>
+      <c r="H114" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4474,7 +4620,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G115" t="inlineStr">
+      <c r="G115" t="inlineStr"/>
+      <c r="H115" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4507,7 +4654,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G116" t="inlineStr">
+      <c r="G116" t="inlineStr"/>
+      <c r="H116" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4540,7 +4688,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G117" t="inlineStr">
+      <c r="G117" t="inlineStr"/>
+      <c r="H117" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4577,7 +4726,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G118" t="inlineStr">
+      <c r="G118" t="inlineStr"/>
+      <c r="H118" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4614,7 +4764,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G119" t="inlineStr">
+      <c r="G119" t="inlineStr"/>
+      <c r="H119" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4651,7 +4802,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G120" t="inlineStr">
+      <c r="G120" t="inlineStr"/>
+      <c r="H120" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4688,7 +4840,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G121" t="inlineStr">
+      <c r="G121" t="inlineStr"/>
+      <c r="H121" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4721,7 +4874,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G122" t="inlineStr">
+      <c r="G122" t="inlineStr"/>
+      <c r="H122" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4758,7 +4912,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G123" t="inlineStr">
+      <c r="G123" t="inlineStr"/>
+      <c r="H123" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4795,7 +4950,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G124" t="inlineStr">
+      <c r="G124" t="inlineStr"/>
+      <c r="H124" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -4828,7 +4984,8 @@
           <t>None</t>
         </is>
       </c>
-      <c r="G125" t="inlineStr">
+      <c r="G125" t="inlineStr"/>
+      <c r="H125" t="inlineStr">
         <is>
           <t>None</t>
         </is>

</xml_diff>

<commit_message>
Spotify updated, Code caught up!
</commit_message>
<xml_diff>
--- a/Book11.xlsx
+++ b/Book11.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>NEW PLAYS March 12, 2025</t>
+          <t>NEW PLAYS September 01, 2025</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -473,17 +473,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>73,425</t>
+          <t>119,494</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-08-09</t>
+          <t>August 9, 2024</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Bineetha Ranjith, Sadanam Jyothish Babu</t>
+          <t>Bineetha Ranjith</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -494,134 +494,6 @@
       <c r="F2" t="inlineStr">
         <is>
           <t>Sundarakalebara</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>https://open.spotify.com/track/2rjoStNmGFO7mHHtkuo0Sc</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>954,522</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2020-04-20</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>IndianRaga, Mayukha Kashyap, Nagaari, Shravan Kumar Ramani, Vinod Krishnan</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>© 2020 IndianRaga</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Rangapuravihara 2.0 - Brindavana Saranga - Rupakam</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>https://open.spotify.com/track/0SofuRi0URqZKKWubjtJlP</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>91,378</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2024-02-08</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Maalavika Sundar, Raj Pandit</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>© 2024 Maalavika Sundar</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Sagara Shayana Vibho</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>https://open.spotify.com/track/5RUjX3giNkPTzABzICs5bH</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1,854,739</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2020-04-20</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Akshay Anantapadmanabhan, IndianRaga, Madhu Iyer, Sri Poornima Krishna Emani</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>© 2020 IndianRaga</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Swagatham Krishna - Mohanam - Adi</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>https://open.spotify.com/track/79thiZzQ1WnQ5wj5cbV3fr</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>604,596</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2021-01-01</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Madhuthva Music</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>© 2021 Madhuthva Music</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>A Tryst with Reethigowla</t>
         </is>
       </c>
     </row>

</xml_diff>